<commit_message>
Updates to compliance tools - testing in progress
</commit_message>
<xml_diff>
--- a/testing_meter_analysis_compliance_report.xlsx
+++ b/testing_meter_analysis_compliance_report.xlsx
@@ -96,13 +96,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,11 +479,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="17" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="29" customWidth="1" min="6" max="6"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -526,7 +526,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>PM8340</t>
+          <t>ION9000</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="inlineStr"/>
     </row>
@@ -559,14 +559,14 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>Voltage accuracy, Harmonics</t>
+          <t>Measurement accuracy, Voltage accuracy</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,7 +590,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="82" customWidth="1" min="1" max="1"/>
-    <col width="70" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="82" customWidth="1" min="4" max="4"/>
   </cols>
@@ -605,14 +605,14 @@
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>Selected Meter: PM8340</t>
+          <t>Selected Meter: ION9000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>Description: Advanced power quality meter with Class A compliance, 512MB memory, and 512 samples/cycle.</t>
+          <t>Description: From PM5000_Series</t>
         </is>
       </c>
     </row>
@@ -648,664 +648,884 @@
     <row r="7">
       <c r="A7" s="8" t="inlineStr">
         <is>
-          <t>LCD graphical display</t>
+          <t>Power quality Meter must be used for all incoming HV and LV Switchgears compartments</t>
         </is>
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
-          <t>Panel Mount with integrated display</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C7" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>The meter has an integrated LCD display, which meets the requirement.</t>
+          <t>The meter specifications do not mention its use in specific switchgear compartments.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="inlineStr">
         <is>
-          <t>Voltage measurement up to 690 VAC Line to Line</t>
+          <t>Colourful LCD graphical display with ability to direct connect to circuits up to 690 VAC Line to Line, eliminating the need for voltage transformers; 5 A nominal current inputs</t>
         </is>
       </c>
       <c r="B8" s="8" t="inlineStr">
         <is>
-          <t>Up to 690 V L-L CAT III</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>The meter supports voltage measurements up to 690 V L-L, which meets the requirement.</t>
+          <t>The meter specifications do not mention its display capabilities or voltage/current input ranges.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
-          <t>Current input: 5 A nominal</t>
+          <t>Complies with IEC 62053 class 0.2S or SAC-SINGLAS certification with passed accuracy class of 0.2 standard</t>
         </is>
       </c>
       <c r="B9" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C9" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a current input capability of 5 A nominal. The specs only indicate voltage measurement capabilities.</t>
+          <t>The meter specifications do not mention any certifications or accuracy classes.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
         <is>
-          <t>IEC62053 class 0.2S or SAC-SINGLAS certification with accuracy class of 0.2 standard</t>
+          <t>Communication via Modbus TCP/IP connection</t>
         </is>
       </c>
       <c r="B10" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 (±0.1% of reading)</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C10" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>The meter has a Class 0.2 accuracy, which is better than the required Class 0.2S. Therefore, it meets the requirement.</t>
+          <t>The meter specifications do not mention communication interfaces.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
         <is>
-          <t>Modbus TCP/IP communication</t>
+          <t>Web server analysis monitoring tools including weekly analysis report, transient/sags/swells events download, export into COMTRADE format, viewing harmonics up to at least 63rd order, flickering analysis, automatic EN50160 report generation</t>
         </is>
       </c>
       <c r="B11" s="8" t="inlineStr">
         <is>
-          <t>Supports Modbus RTU, Modbus TCP, DNP3, IEC 61850.</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C11" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>The meter supports Modbus TCP/IP through its support for Modbus TCP.</t>
+          <t>The meter specifications do not mention any web server or specific monitoring tools.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
-          <t>Web server analysis monitoring tools for power quality analysis</t>
+          <t>Class A Power Analyser</t>
         </is>
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>Onboard web server for access to data, reports, and alarms.</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>The meter has an onboard web server, which allows for web-based analysis and monitoring.</t>
+          <t>The meter specifications do not mention power analyser capabilities.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="inlineStr">
         <is>
-          <t>Weekly analysis report</t>
+          <t>Monitoring quality in accordance with DIN EN 50160</t>
         </is>
       </c>
       <c r="B13" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C13" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C13" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for generating weekly analysis reports. The specs only indicate an onboard web server for data access.</t>
+          <t>The meter specifications do not mention compliance with DIN EN 50160.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="inlineStr">
         <is>
-          <t>Transient / Sags/ Swells events download</t>
+          <t>Measurement accuracy according to IEC 62053-22 Cl 0.2S</t>
         </is>
       </c>
       <c r="B14" s="8" t="inlineStr">
         <is>
-          <t>Disturbance detection and capture on any voltage or current channel.</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C14" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>The meter has the capability to detect and capture transient events, including sags and swells.</t>
+          <t>The meter specifications do not mention measurement accuracy.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="inlineStr">
         <is>
-          <t>Export event information into COMTRADE format</t>
+          <t>Support for IEC 61850</t>
         </is>
       </c>
       <c r="B15" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C15" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C15" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for exporting event information into COMTRADE format. The specs only indicate disturbance detection and capture.</t>
+          <t>The meter specifications do not mention support for IEC 61850.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="inlineStr">
         <is>
-          <t>Viewing harmonics up to at least 63rd order</t>
+          <t>8GB Internal Memory</t>
         </is>
       </c>
       <c r="B16" s="8" t="inlineStr">
         <is>
-          <t>Harmonics: Class 1 (IEC 61000-4-7)</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C16" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>The meter supports harmonic analysis up to the 63rd order, which meets the requirement.</t>
+          <t>The meter specifications do not mention internal memory capacity.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="inlineStr">
         <is>
-          <t>Flickering and rapid voltage changes analysis</t>
+          <t>SNTP Time sync available</t>
         </is>
       </c>
       <c r="B17" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C17" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C17" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for analyzing flickering and rapid voltage changes. The specs only indicate disturbance detection and capture.</t>
+          <t>The meter specifications do not mention time synchronization capabilities.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
-          <t>Automatic weekly EN50160 report generation</t>
+          <t>8 Digital Inputs (DI), 4 Relay Outputs (RO), 2 Digital Outputs (DO)</t>
         </is>
       </c>
       <c r="B18" s="8" t="inlineStr">
         <is>
-          <t>Onboard PQ compliance reports for EN 50160 and IEEE 519 (PM83xx).</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C18" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>The meter has the capability to generate EN50160 reports automatically.</t>
+          <t>The meter specifications do not mention digital input/output capabilities.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="inlineStr">
         <is>
-          <t>Class A Power Analyser</t>
+          <t>Operating temperature -10°C to +55°C</t>
         </is>
       </c>
       <c r="B19" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C19" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C19" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for Class A power analysis. The specs only indicate voltage and current accuracy.</t>
+          <t>The meter specifications do not mention operating temperature range.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>Monitoring in accordance with DIN EN 50160</t>
+          <t>IP52 at front; IP30 at Side and Back</t>
         </is>
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>Onboard PQ compliance reports for EN 50160 and IEEE 519 (PM83xx).</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C20" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>The meter supports monitoring in accordance with DIN EN 50160 through its onboard PQ compliance reports.</t>
+          <t>The meter specifications do not mention IP ratings.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
-          <t>Measurement accuracy according to IEC62053-22 Cl 0.2S</t>
+          <t>Measured circuit breaker ON/OFF/TRIP status linked for status monitoring</t>
         </is>
       </c>
       <c r="B21" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 (±0.1% of reading)</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C21" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>The meter has a Class 0.2 accuracy, which is better than the required Class 0.2S. Therefore, it meets the requirement.</t>
+          <t>The meter specifications do not mention circuit breaker status monitoring capabilities.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="inlineStr">
         <is>
-          <t>Instantaneous values, L-N voltage, L-L voltage, frequency, power, power factor, THDV, THDI</t>
+          <t>THD and TDD up to 63rd order</t>
         </is>
       </c>
       <c r="B22" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C22" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C22" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D22" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for measuring instantaneous values, L-N voltage, L-L voltage, frequency, power, power factor, THDV, and THDI. The specs only indicate voltage and current accuracy.</t>
+          <t>The meter specifications do not mention THD/TDD measurement capabilities.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="inlineStr">
         <is>
-          <t>Support for IEC61850</t>
+          <t>EN50160 statistic function</t>
         </is>
       </c>
       <c r="B23" s="8" t="inlineStr">
         <is>
-          <t>Communications.protocols: Modbus RTU, Modbus TCP, DNP3, IEC 61850.</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C23" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>The meter supports IEC61850 through its support for the IEC 61850 protocol.</t>
+          <t>The meter specifications do not mention EN50160 statistics.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
-          <t>Internal Memory: 8GB</t>
+          <t>Unbalance Voltage-, current- and zero sequence</t>
         </is>
       </c>
       <c r="B24" s="8" t="inlineStr">
         <is>
-          <t>Up to 512 MB onboard memory.</t>
-        </is>
-      </c>
-      <c r="C24" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C24" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>The meter has an internal memory of up to 512 MB, which is less than the required 8 GB. Therefore, it does not meet the requirement.</t>
+          <t>The meter specifications do not mention unbalance measurement capabilities.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="inlineStr">
         <is>
-          <t>SNTP Time sync available</t>
+          <t>Voltage/Freq. Deviation Setpoint alarm and record</t>
         </is>
       </c>
       <c r="B25" s="8" t="inlineStr">
         <is>
-          <t>Time_sync: GPS time synchronization via RS-485 port.</t>
-        </is>
-      </c>
-      <c r="C25" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C25" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>The meter supports GPS time synchronization via RS-485, but it does not mention SNTP time synchronization. Therefore, it does not meet the requirement.</t>
+          <t>The meter specifications do not mention deviation setpoint alarms or records.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
         <is>
-          <t>Digital Inputs (DI): 8</t>
+          <t>Rapid Voltage Alteration Trigger DO point, waveform record</t>
         </is>
       </c>
       <c r="B26" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C26" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for digital inputs. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention rapid voltage alteration triggers or waveforms.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="inlineStr">
         <is>
-          <t>Relay Outputs (RO): 4</t>
+          <t>High resolution failure record with 1024 points / cycle</t>
         </is>
       </c>
       <c r="B27" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C27" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C27" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for relay outputs. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention high resolution failure records.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>Digital Outputs (DO): 2</t>
+          <t>Support for up to 1024 PQ Records with time resolution of 1ms</t>
         </is>
       </c>
       <c r="B28" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C28" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C28" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for digital outputs. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention PQ record support.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="inlineStr">
         <is>
-          <t>Operating temperature range -10°C to +55°C</t>
+          <t>Voltage Sag/Swell Waveform record available</t>
         </is>
       </c>
       <c r="B29" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C29" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C29" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention an operating temperature range. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention voltage sag/swell waveform records.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
-          <t>IP rating: IP52 at front; IP30 at Side and Back</t>
+          <t>20µs for transient disturbance record</t>
         </is>
       </c>
       <c r="B30" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C30" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C30" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention an IP rating. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention transient disturbance records.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="inlineStr">
         <is>
-          <t>Linkage of circuit breaker status to PQM for status monitoring</t>
+          <t>Configurable waveform recording mode: 50 cycles, 100 cycles, 200 cycles, 400 cycles, 800 cycles, 1600 cycles, 3200 cycles</t>
         </is>
       </c>
       <c r="B31" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C31" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C31" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for linking circuit breaker status. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention configurable waveform recording modes.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="inlineStr">
         <is>
-          <t>THD and TDD up to 63rd order</t>
+          <t>Sag Source Location locate power supply side load side abnormal and fault</t>
         </is>
       </c>
       <c r="B32" s="8" t="inlineStr">
         <is>
-          <t>Harmonics: Class 1 (IEC 61000-4-7)</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C32" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>The meter supports harmonic analysis up to the 63rd order, which meets the requirement.</t>
+          <t>The meter specifications do not mention sag source location capabilities.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="inlineStr">
         <is>
-          <t>EN50160 statistic function</t>
+          <t>ITIC Curve/SEMI F47/SARFI Index analysis included</t>
         </is>
       </c>
       <c r="B33" s="8" t="inlineStr">
         <is>
-          <t>Onboard PQ compliance reports for EN 50160 and IEEE 519 (PM83xx).</t>
+          <t>Not specified in the meter specifications</t>
         </is>
       </c>
       <c r="C33" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>The meter supports the EN50160 statistic function through its onboard PQ compliance reports.</t>
+          <t>The meter specifications do not mention ITIC curve or SEMI F47/SARFI index analysis.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="inlineStr">
         <is>
-          <t>Unbalance Voltage-, current- and zero sequence</t>
+          <t>Voltage Accuracy ±0.1%</t>
         </is>
       </c>
       <c r="B34" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C34" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C34" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for unbalance voltage, current, and zero sequence analysis. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention voltage accuracy.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
         <is>
-          <t>Flickering and rapid voltage changes analysis</t>
+          <t>Current Accuracy ±0.1%</t>
         </is>
       </c>
       <c r="B35" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C35" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C35" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D35" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for analyzing flickering and rapid voltage changes. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
+          <t>The meter specifications do not mention current accuracy.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
         <is>
-          <t>Class A Power Analyser</t>
+          <t>Frequency Accuracy ±0.005Hz</t>
         </is>
       </c>
       <c r="B36" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly stated in the specs</t>
-        </is>
-      </c>
-      <c r="C36" s="10" t="inlineStr">
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C36" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
         <is>
-          <t>The meter specifications do not mention a feature for Class A power analysis. The specs only indicate support for Modbus RTU, Modbus TCP, DNP3, and IEC 61850.</t>
-        </is>
-      </c>
-    </row>
-    <row r="37"/>
+          <t>The meter specifications do not mention frequency accuracy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>Active Power Accuracy ±0.2%</t>
+        </is>
+      </c>
+      <c r="B37" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C37" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D37" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention active power accuracy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="8" t="inlineStr">
+        <is>
+          <t>Active Energy Class 0.2s</t>
+        </is>
+      </c>
+      <c r="B38" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C38" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D38" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention active energy class.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="8" t="inlineStr">
+        <is>
+          <t>Reactive Energy Class 2</t>
+        </is>
+      </c>
+      <c r="B39" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C39" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D39" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention reactive energy class.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="8" t="inlineStr">
+        <is>
+          <t>Power Factor Accuracy ±0.5%</t>
+        </is>
+      </c>
+      <c r="B40" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C40" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D40" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention power factor accuracy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="8" t="inlineStr">
+        <is>
+          <t>Voltage Unbalance ±0.1%</t>
+        </is>
+      </c>
+      <c r="B41" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C41" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D41" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention voltage unbalance.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="inlineStr">
+        <is>
+          <t>Current Unbalance ±0.5%</t>
+        </is>
+      </c>
+      <c r="B42" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C42" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D42" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention current unbalance.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="inlineStr">
+        <is>
+          <t>Voltage Deviation ±0.1%</t>
+        </is>
+      </c>
+      <c r="B43" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C43" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D43" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention voltage deviation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="inlineStr">
+        <is>
+          <t>Frequency Deviation ±0.005Hz</t>
+        </is>
+      </c>
+      <c r="B44" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C44" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D44" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention frequency deviation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="8" t="inlineStr">
+        <is>
+          <t>Flicker ±5%</t>
+        </is>
+      </c>
+      <c r="B45" s="8" t="inlineStr">
+        <is>
+          <t>Not specified in the meter specifications</t>
+        </is>
+      </c>
+      <c r="C45" s="9" t="inlineStr">
+        <is>
+          <t>❌ Non-compliant</t>
+        </is>
+      </c>
+      <c r="D45" s="8" t="inlineStr">
+        <is>
+          <t>The meter specifications do not mention flicker measurement capabilities.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="n"/>
+      <c r="B46" s="8" t="n"/>
+      <c r="C46" s="8" t="n"/>
+      <c r="D46" s="8" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="10" t="inlineStr">
+        <is>
+          <t>Potential Compliance Issues:</t>
+        </is>
+      </c>
+      <c r="B47" s="8" t="n"/>
+      <c r="C47" s="8" t="n"/>
+      <c r="D47" s="8" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>- No specific certification for revenue metering mentioned</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1317,7 +1537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1326,7 +1546,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="82" customWidth="1" min="1" max="1"/>
-    <col width="61" customWidth="1" min="2" max="2"/>
+    <col width="29" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="82" customWidth="1" min="4" max="4"/>
   </cols>
@@ -1348,7 +1568,7 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>Description: Advanced power quality meter with Class A compliance, 512MB memory, and 512 samples/cycle.</t>
+          <t>Description: Standard power quality meter with integrated display, 512 MB memory, and 256 samples/cycle.</t>
         </is>
       </c>
     </row>
@@ -1389,39 +1609,39 @@
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 S (±0.1% of reading)</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
+          <t>Class 0.5 S (±1%)</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>✅ Exceeds</t>
         </is>
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 S (±0.1%) EXCEEDS the required IEC62053-22 Cl 0.5S accuracy</t>
+          <t>The meter's Class 0.5 S (±1%) EXCEEDS the required IEC62053-22 Cl 0.5S accuracy</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="inlineStr">
         <is>
-          <t>Instantaneous values, L-N voltage, L-L voltage, frequency, power, power factor, THDV, THDI</t>
+          <t>Instantaneous values (L-N voltage, L-L voltage, frequency, power, power factor, THDV, THDI)</t>
         </is>
       </c>
       <c r="B8" s="8" t="inlineStr">
         <is>
-          <t>All specified features are supported by the meter.</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>The meter supports all the required instantaneous measurements and power quality parameters.</t>
+          <t>The meter specifications do not mention support for instantaneous values.</t>
         </is>
       </c>
     </row>
@@ -1433,61 +1653,61 @@
       </c>
       <c r="B9" s="8" t="inlineStr">
         <is>
-          <t>Class 0.5 S (±1%) with individual harmonics up to the 63rd.</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C9" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>The meter supports harmonics up to the 63rd order, which EXCEEDS the requirement.</t>
+          <t>The meter specifications do not mention support for harmonics up to 63rd order.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
         <is>
-          <t>Memory Recording for energy, demand, max demand &amp; max/min record</t>
+          <t>Memory recording for energy, demand, max demand &amp; max/min record</t>
         </is>
       </c>
       <c r="B10" s="8" t="inlineStr">
         <is>
-          <t>Data logging is available on PM5300 and PM5500 series.</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C10" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>The meter has data logging capabilities, which meets the requirement.</t>
+          <t>The meter specifications do not mention memory recording capabilities.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
         <is>
-          <t>Real time clock</t>
+          <t>Real-time clock</t>
         </is>
       </c>
       <c r="B11" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C11" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C11" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have a real-time clock feature as specified.</t>
+          <t>The meter specifications do not mention a real-time clock feature.</t>
         </is>
       </c>
     </row>
@@ -1499,127 +1719,127 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>RS-485 Modbus (all series).</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>✅ Compliant</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>The meter supports RS-485 Modbus, which is a form of Modbus RTU communication.</t>
+          <t>The meter specifications do not mention built-in Modbus RTU communication capability.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="inlineStr">
         <is>
-          <t>6.4kHz sampling (128 Samples/cycle)</t>
+          <t>Sampling rate: 6.4kHz (128 Samples/cycle)</t>
         </is>
       </c>
       <c r="B13" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C13" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C13" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have 6.4kHz sampling capability as specified.</t>
+          <t>The meter specifications do not mention a sampling rate of 6.4kHz.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="inlineStr">
         <is>
-          <t>Operating temperature -25°C to +55°C</t>
+          <t>Operating temperature range: -25°C to +55°C</t>
         </is>
       </c>
       <c r="B14" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C14" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>The meter's operating temperature range is not specified, so it cannot be determined if it complies.</t>
+          <t>The meter specifications do not mention an operating temperature range of -25°C to +55°C.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="inlineStr">
         <is>
-          <t>Apparent power accuracy ±0.5%</t>
+          <t>Apparent power accuracy: ±0.5%</t>
         </is>
       </c>
       <c r="B15" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 S (±0.1% of reading)</t>
-        </is>
-      </c>
-      <c r="C15" s="9" t="inlineStr">
+          <t>Class 0.5 S (±1%)</t>
+        </is>
+      </c>
+      <c r="C15" s="11" t="inlineStr">
         <is>
           <t>✅ Exceeds</t>
         </is>
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 S (±0.1%) EXCEEDS the required ±0.5% accuracy.</t>
+          <t>The meter's Class 0.5 S (±1%) EXCEEDS the required ±0.5% apparent power accuracy</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="inlineStr">
         <is>
-          <t>Reactive power accuracy ±1%</t>
+          <t>Reactive power accuracy: ±1%</t>
         </is>
       </c>
       <c r="B16" s="8" t="inlineStr">
         <is>
-          <t>Class 1 (PM55xx) / Class 2 (PM51xx/53xx)</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C16" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 1 (±0.5%) EXCEEDS the required ±1% accuracy.</t>
+          <t>The meter specifications do not mention reactive power accuracy.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="inlineStr">
         <is>
-          <t>Power factor accuracy ±0.01</t>
+          <t>Power factor accuracy: ±0.01</t>
         </is>
       </c>
       <c r="B17" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 S (±0.1% of reading)</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C17" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 S (±0.1%) EXCEEDS the required ±0.01 accuracy.</t>
+          <t>The meter specifications do not mention power factor accuracy.</t>
         </is>
       </c>
     </row>
@@ -1631,17 +1851,17 @@
       </c>
       <c r="B18" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 S (±0.1% of reading)</t>
-        </is>
-      </c>
-      <c r="C18" s="9" t="inlineStr">
+          <t>Class 0.5 S (±1%)</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="inlineStr">
         <is>
           <t>✅ Exceeds</t>
         </is>
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 S (±0.1%) EXCEEDS the required IEC62053-22 Cl 0.5S accuracy.</t>
+          <t>The meter's Class 0.5 S (±1%) EXCEEDS the required IEC62053-22 Class 0.5S accuracy</t>
         </is>
       </c>
     </row>
@@ -1653,303 +1873,303 @@
       </c>
       <c r="B19" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 S (±0.1% of reading)</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C19" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 S (±0.1%) EXCEEDS the required IEC 61557-12 Cl 0.5 accuracy.</t>
+          <t>The meter specifications do not mention active energy accuracy according to IEC 61557-12 Class 0.5.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>THD accuracy ±1%</t>
+          <t>Total harmonic distortion (THD) accuracy: ±1%</t>
         </is>
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>Class 0.5 S (±1%)</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C20" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.5 S (±1%) EXCEEDS the required ±1% accuracy.</t>
+          <t>The meter specifications do not mention THD accuracy.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
-          <t>Voltage VL-N accuracy ±0.2%</t>
+          <t>Voltage accuracy: VL-N ±0.2%, VL-L ±0.2%</t>
         </is>
       </c>
       <c r="B21" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 (±0.1% of reading)</t>
-        </is>
-      </c>
-      <c r="C21" s="9" t="inlineStr">
+          <t>Class 0.5 S (±1%)</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
         <is>
           <t>✅ Exceeds</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 (±0.1%) EXCEEDS the required ±0.2% accuracy.</t>
+          <t>The meter's Class 0.5 S (±1%) EXCEEDS the required ±0.2% voltage accuracy</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="inlineStr">
         <is>
-          <t>Current accuracy ±0.2%</t>
+          <t>Current accuracy: ±0.2%</t>
         </is>
       </c>
       <c r="B22" s="8" t="inlineStr">
         <is>
-          <t>Class 0.2 (±0.15% of reading)</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C22" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D22" s="8" t="inlineStr">
         <is>
-          <t>The meter's Class 0.2 (±0.15%) EXCEEDS the required ±0.2% accuracy.</t>
+          <t>The meter specifications do not mention current accuracy.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="inlineStr">
         <is>
-          <t>Frequency accuracy ±0.1%</t>
+          <t>Frequency accuracy: ±0.1%</t>
         </is>
       </c>
       <c r="B23" s="8" t="inlineStr">
         <is>
-          <t>±0.02 Hz</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C23" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>The meter's ±0.02 Hz EXCEEDS the required ±0.1% accuracy.</t>
+          <t>The meter specifications do not mention frequency accuracy.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
-          <t>Electrostatic Discharge compliance with IEC 61000-4-2</t>
+          <t>Electrostatic Discharge immunity IEC 61000-4-2</t>
         </is>
       </c>
       <c r="B24" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C24" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C24" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have Electrostatic Discharge compliance as specified.</t>
+          <t>The meter specifications do not mention electrostatic discharge immunity.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="inlineStr">
         <is>
-          <t>Immunity to Radiated Fields compliance with IEC 61000-4-3</t>
+          <t>Immunity to radiated fields IEC 61000-4-3</t>
         </is>
       </c>
       <c r="B25" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C25" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C25" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have immunity to radiated fields as specified.</t>
+          <t>The meter specifications do not mention immunity to radiated fields.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
         <is>
-          <t>Immunity to Fast Transients compliance with IEC 61000-4-4</t>
+          <t>Immunity to fast transients IEC 61000-4-4</t>
         </is>
       </c>
       <c r="B26" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C26" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have immunity to fast transients as specified.</t>
+          <t>The meter specifications do not mention immunity to fast transients.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="inlineStr">
         <is>
-          <t>Immunity to Impulse Waves compliance with IEC 61000-4-5</t>
+          <t>Immunity to impulse waves IEC 61000-4-5</t>
         </is>
       </c>
       <c r="B27" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C27" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C27" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have immunity to impulse waves as specified.</t>
+          <t>The meter specifications do not mention immunity to impulse waves.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>Conducted Immunity compliance with IEC 61000-4-6</t>
+          <t>Conducted immunity IEC 61000-4-6</t>
         </is>
       </c>
       <c r="B28" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C28" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C28" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have conducted immunity as specified.</t>
+          <t>The meter specifications do not mention conducted immunity.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="inlineStr">
         <is>
-          <t>Immunity to Voltage Dips compliance with IEC 61000-4-11</t>
+          <t>Immunity to magnetic fields IEC 61000-4-8</t>
         </is>
       </c>
       <c r="B29" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C29" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C29" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have immunity to voltage dips as specified.</t>
+          <t>The meter specifications do not mention immunity to magnetic fields.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
-          <t>Radiated Emissions Class A compliance with EN55011</t>
+          <t>Immunity to voltage dips IEC 61000-4-11</t>
         </is>
       </c>
       <c r="B30" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C30" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C30" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have radiated emissions compliance as specified.</t>
+          <t>The meter specifications do not mention immunity to voltage dips.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="inlineStr">
         <is>
-          <t>Harmonics compliance with IEC 61000-3-2</t>
+          <t>Radiated emissions EN55011 Class A</t>
         </is>
       </c>
       <c r="B31" s="8" t="inlineStr">
         <is>
-          <t>Class 0.5 S (±1%) with individual harmonics up to the 63rd.</t>
+          <t>Not specified in meter data</t>
         </is>
       </c>
       <c r="C31" s="9" t="inlineStr">
         <is>
-          <t>✅ Exceeds</t>
+          <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>The meter supports harmonics up to the 63rd order, which EXCEEDS the requirement.</t>
+          <t>The meter specifications do not mention radiated emissions.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="inlineStr">
         <is>
-          <t>Certifications: SACSINGLAS, third party lab certifications</t>
+          <t>Harmonics compliance with IEC 61000-3-2</t>
         </is>
       </c>
       <c r="B32" s="8" t="inlineStr">
         <is>
-          <t>Not explicitly mentioned in the specifications.</t>
-        </is>
-      </c>
-      <c r="C32" s="10" t="inlineStr">
+          <t>Not specified in meter data</t>
+        </is>
+      </c>
+      <c r="C32" s="9" t="inlineStr">
         <is>
           <t>❌ Non-compliant</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>The meter does not have specific certifications as specified.</t>
+          <t>The meter specifications do not mention harmonics compliance.</t>
         </is>
       </c>
     </row>
@@ -1960,7 +2180,7 @@
       <c r="D33" s="8" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="11" t="inlineStr">
+      <c r="A34" s="10" t="inlineStr">
         <is>
           <t>Areas Exceeding Requirements:</t>
         </is>
@@ -1972,7 +2192,7 @@
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
         <is>
-          <t>- Voltage accuracy</t>
+          <t>- Measurement accuracy</t>
         </is>
       </c>
       <c r="B35" s="8" t="n"/>
@@ -1982,7 +2202,7 @@
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
         <is>
-          <t>- Harmonics</t>
+          <t>- Voltage accuracy</t>
         </is>
       </c>
       <c r="B36" s="8" t="n"/>
@@ -1990,7 +2210,7 @@
       <c r="D36" s="8" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="11" t="inlineStr">
+      <c r="A37" s="10" t="inlineStr">
         <is>
           <t>Potential Compliance Issues:</t>
         </is>
@@ -2000,69 +2220,9 @@
       <c r="D37" s="8" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="8" t="inlineStr">
-        <is>
-          <t>- No real-time clock feature</t>
-        </is>
-      </c>
-      <c r="B38" s="8" t="n"/>
-      <c r="C38" s="8" t="n"/>
-      <c r="D38" s="8" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="8" t="inlineStr">
-        <is>
-          <t>- No 6.4kHz sampling capability</t>
-        </is>
-      </c>
-      <c r="B39" s="8" t="n"/>
-      <c r="C39" s="8" t="n"/>
-      <c r="D39" s="8" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="8" t="inlineStr">
-        <is>
-          <t>- Operating temperature range not specified</t>
-        </is>
-      </c>
-      <c r="B40" s="8" t="n"/>
-      <c r="C40" s="8" t="n"/>
-      <c r="D40" s="8" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="8" t="inlineStr">
-        <is>
-          <t>- Electrostatic Discharge compliance not mentioned</t>
-        </is>
-      </c>
-      <c r="B41" s="8" t="n"/>
-      <c r="C41" s="8" t="n"/>
-      <c r="D41" s="8" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="8" t="inlineStr">
-        <is>
-          <t>- Immunity to radiated fields, fast transients, impulse waves, conducted immunity, and voltage dips not mentioned</t>
-        </is>
-      </c>
-      <c r="B42" s="8" t="n"/>
-      <c r="C42" s="8" t="n"/>
-      <c r="D42" s="8" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="8" t="inlineStr">
-        <is>
-          <t>- Radiated emissions compliance not mentioned</t>
-        </is>
-      </c>
-      <c r="B43" s="8" t="n"/>
-      <c r="C43" s="8" t="n"/>
-      <c r="D43" s="8" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>- Specific certifications for revenue metering not mentioned</t>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>- No specific certification for revenue metering mentioned</t>
         </is>
       </c>
     </row>

</xml_diff>